<commit_message>
Dokumentation - Kalibrering af måleenhed
</commit_message>
<xml_diff>
--- a/Maaleenhed/Notater/3 maj - Volampere kredsløb/Kalibrering.xlsx
+++ b/Maaleenhed/Notater/3 maj - Volampere kredsløb/Kalibrering.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28315"/>
+  <workbookPr codeName="ThisWorkbook" checkCompatibility="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Soren/Desktop/Projekt/Maaleenhed/Notater/3 maj - Vol:ampere kredsløb/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Soren/Desktop/EE-projekt-4-gruppe-1/Maaleenhed/Notater/3 maj - Volampere kredsløb/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Ark2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>Kaliberring</t>
   </si>
@@ -47,9 +48,6 @@
     <t xml:space="preserve">Spænding </t>
   </si>
   <si>
-    <t>rms-værdier</t>
-  </si>
-  <si>
     <t>kg</t>
   </si>
   <si>
@@ -93,6 +91,96 @@
   </si>
   <si>
     <t>mV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Måling nr. </t>
+  </si>
+  <si>
+    <t>% Table generated by Excel2LaTeX from sheet 'Ark1'</t>
+  </si>
+  <si>
+    <t>\begin{table}[htbp]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  \centering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  \caption{Add caption}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    \begin{tabular}{rrrrr}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    \toprule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          &amp; \multicolumn{1}{l}{Faktiske værdier} &amp;       &amp; \multicolumn{1}{l}{Måleenhed} &amp;  \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    \multicolumn{1}{l}{Måling nr. } &amp; \multicolumn{1}{l}{Spænding} &amp; \multicolumn{1}{l}{Strøm} &amp; \multicolumn{1}{l}{Spænding } &amp; \multicolumn{1}{l}{Strøm} \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    \midrule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    1     &amp; 0     &amp; 0     &amp; 0     &amp; 0 \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    2     &amp; 500   &amp; 50    &amp; 93    &amp; 152 \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    3     &amp; 1000  &amp; 100   &amp; 185   &amp; 308 \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    4     &amp; 1509  &amp; 150   &amp; 276   &amp; 462 \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    5     &amp; 2008  &amp; 199   &amp; 368   &amp; 610 \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    6     &amp; 2503  &amp; 250   &amp; 460   &amp; 764 \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    7     &amp; 2999  &amp; 299   &amp; 553   &amp; 912 \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    8     &amp; 3502  &amp; 350   &amp; 645   &amp; 1069 \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    9     &amp; 3808  &amp; 399   &amp; 699   &amp; 1216 \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    10    &amp; 4006  &amp; 450   &amp; 736   &amp; 1370 \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    11    &amp; 4505  &amp; 500   &amp; 828   &amp; 1518 \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    12    &amp; 5000  &amp;       &amp; 918   &amp;  \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    13    &amp; 5499  &amp;       &amp; 1009  &amp;  \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    14    &amp; 6000  &amp;       &amp; 1111  &amp;  \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    15    &amp; 6505  &amp;       &amp; 1197  &amp;  \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    16    &amp; 7006  &amp;       &amp; 1284  &amp;  \\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    \bottomrule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    \end{tabular}%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  \label{tab:addlabel}%</t>
+  </si>
+  <si>
+    <t>\end{table}%</t>
   </si>
 </sst>
 </file>
@@ -141,7 +229,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -164,11 +252,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -176,6 +291,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -256,10 +375,43 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-0.134733978164882"/>
-                  <c:y val="0.00827617074181517"/>
+                  <c:x val="-0.0969781302959385"/>
+                  <c:y val="0.0468537803742274"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 5,4391x - 0,6016</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>R² = 0,99996</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -292,10 +444,10 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ark1'!$E$8:$E$25</c:f>
+              <c:f>'Ark1'!$D$8:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
                 </c:pt>
@@ -452,10 +604,43 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="0.0328959776806816"/>
-                  <c:y val="-0.0543945296311645"/>
+                  <c:x val="-0.00697928315329544"/>
+                  <c:y val="-0.0470516891033782"/>
                 </c:manualLayout>
               </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 0,3291x - 1,0288</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>R² = 0,99998</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -488,7 +673,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'Ark1'!$F$8:$F$23</c:f>
+              <c:f>'Ark1'!$E$8:$E$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
@@ -580,11 +765,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="749949440"/>
-        <c:axId val="750271568"/>
+        <c:axId val="1078144720"/>
+        <c:axId val="1078147040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="749949440"/>
+        <c:axId val="1078144720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -618,6 +803,63 @@
             <a:effectLst/>
           </c:spPr>
         </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>Måleenhed</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="da-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -654,12 +896,765 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="750271568"/>
+        <c:crossAx val="1078147040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="750271568"/>
+        <c:axId val="1078147040"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>Faktiske værdier</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="da-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1078144720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.206459690342514"/>
+          <c:y val="0.925267779865318"/>
+          <c:w val="0.549013269388179"/>
+          <c:h val="0.0506035338076038"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="da-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="da-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="da-DK"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Spænding</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.0969781302959385"/>
+                  <c:y val="0.0468537803742274"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 5,4391x - 0,6016</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>R² = 0,99996</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="da-DK"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ark1'!$D$8:$D$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>93.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>185.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>276.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>368.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>460.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>553.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>645.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>699.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>736.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>828.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>918.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1009.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1111.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1197.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1284.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ark1'!$B$8:$B$25</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="18"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1509.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2008.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2503.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2999.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3502.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3808.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4006.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4505.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5000.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5499.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6000.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>6505.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>7006.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Strøm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00697928315329544"/>
+                  <c:y val="-0.0470516891033782"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:pPr>
+                      <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="65000"/>
+                            <a:lumOff val="35000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                        <a:latin typeface="+mn-lt"/>
+                        <a:ea typeface="+mn-ea"/>
+                        <a:cs typeface="+mn-cs"/>
+                      </a:defRPr>
+                    </a:pPr>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>y = 0,3291x - 1,0288</a:t>
+                    </a:r>
+                    <a:br>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                    </a:br>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                      <a:t>R² = 0,99998</a:t>
+                    </a:r>
+                    <a:endParaRPr lang="en-US" sz="1400"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="da-DK"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Ark1'!$E$8:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>152.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>308.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>462.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>610.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>764.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>912.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1069.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1216.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1370.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1518.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Ark1'!$C$8:$C$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>199.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>299.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>350.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>399.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>450.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>500.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1161688096"/>
+        <c:axId val="1161690576"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1161688096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1161690576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1161690576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -749,6 +1744,7 @@
             </a:p>
           </c:txPr>
         </c:title>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -785,7 +1781,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="749949440"/>
+        <c:crossAx val="1161688096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -906,7 +1902,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1434,13 +2986,50 @@
     <xdr:to>
       <xdr:col>17</xdr:col>
       <xdr:colOff>520700</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Diagram 1"/>
         <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagram 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -1720,10 +3309,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:M87"/>
+  <sheetPr codeName="Ark1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A3:P87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74:M74"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="P30" sqref="P30:P58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1731,304 +3321,389 @@
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>1</v>
+      </c>
+      <c r="B8" s="9">
+        <v>0</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0</v>
+      </c>
+      <c r="E8" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>2</v>
+      </c>
+      <c r="B9" s="9">
+        <v>500</v>
+      </c>
+      <c r="C9" s="9">
+        <v>50</v>
+      </c>
+      <c r="D9" s="9">
+        <v>93</v>
+      </c>
+      <c r="E9" s="9">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>3</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1000</v>
+      </c>
+      <c r="C10" s="9">
+        <v>100</v>
+      </c>
+      <c r="D10" s="9">
+        <v>185</v>
+      </c>
+      <c r="E10" s="9">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>4</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1509</v>
+      </c>
+      <c r="C11" s="9">
+        <v>150</v>
+      </c>
+      <c r="D11" s="9">
+        <v>276</v>
+      </c>
+      <c r="E11" s="9">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>5</v>
+      </c>
+      <c r="B12" s="9">
+        <v>2008</v>
+      </c>
+      <c r="C12" s="9">
+        <v>199</v>
+      </c>
+      <c r="D12" s="9">
+        <v>368</v>
+      </c>
+      <c r="E12" s="9">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" t="s">
-        <v>5</v>
-      </c>
-      <c r="F7" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>2</v>
-      </c>
-      <c r="B9">
+      <c r="B13" s="9">
+        <v>2503</v>
+      </c>
+      <c r="C13" s="9">
+        <v>250</v>
+      </c>
+      <c r="D13" s="9">
+        <v>460</v>
+      </c>
+      <c r="E13" s="9">
+        <v>764</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
+        <v>7</v>
+      </c>
+      <c r="B14" s="9">
+        <v>2999</v>
+      </c>
+      <c r="C14" s="9">
+        <v>299</v>
+      </c>
+      <c r="D14" s="9">
+        <v>553</v>
+      </c>
+      <c r="E14" s="9">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>8</v>
+      </c>
+      <c r="B15" s="9">
+        <v>3502</v>
+      </c>
+      <c r="C15" s="9">
+        <v>350</v>
+      </c>
+      <c r="D15" s="9">
+        <v>645</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>9</v>
+      </c>
+      <c r="B16" s="9">
+        <v>3808</v>
+      </c>
+      <c r="C16" s="9">
+        <v>399</v>
+      </c>
+      <c r="D16" s="9">
+        <v>699</v>
+      </c>
+      <c r="E16" s="9">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>10</v>
+      </c>
+      <c r="B17" s="9">
+        <v>4006</v>
+      </c>
+      <c r="C17" s="9">
+        <v>450</v>
+      </c>
+      <c r="D17" s="9">
+        <v>736</v>
+      </c>
+      <c r="E17" s="9">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>11</v>
+      </c>
+      <c r="B18" s="9">
+        <v>4505</v>
+      </c>
+      <c r="C18" s="9">
         <v>500</v>
       </c>
-      <c r="C9">
-        <v>50</v>
-      </c>
-      <c r="E9">
-        <v>93</v>
-      </c>
-      <c r="F9">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>3</v>
-      </c>
-      <c r="B10">
-        <v>1000</v>
-      </c>
-      <c r="C10">
-        <v>100</v>
-      </c>
-      <c r="E10">
-        <v>185</v>
-      </c>
-      <c r="F10">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>4</v>
-      </c>
-      <c r="B11">
-        <v>1509</v>
-      </c>
-      <c r="C11">
-        <v>150</v>
-      </c>
-      <c r="E11">
-        <v>276</v>
-      </c>
-      <c r="F11">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>5</v>
-      </c>
-      <c r="B12">
-        <v>2008</v>
-      </c>
-      <c r="C12">
-        <v>199</v>
-      </c>
-      <c r="E12">
-        <v>368</v>
-      </c>
-      <c r="F12">
-        <v>610</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>6</v>
-      </c>
-      <c r="B13">
-        <v>2503</v>
-      </c>
-      <c r="C13">
-        <v>250</v>
-      </c>
-      <c r="E13">
-        <v>460</v>
-      </c>
-      <c r="F13">
-        <v>764</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>2999</v>
-      </c>
-      <c r="C14">
-        <v>299</v>
-      </c>
-      <c r="E14">
-        <v>553</v>
-      </c>
-      <c r="F14">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>8</v>
-      </c>
-      <c r="B15">
-        <v>3502</v>
-      </c>
-      <c r="C15">
-        <v>350</v>
-      </c>
-      <c r="E15">
-        <v>645</v>
-      </c>
-      <c r="F15">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>9</v>
-      </c>
-      <c r="B16">
-        <v>3808</v>
-      </c>
-      <c r="C16">
-        <v>399</v>
-      </c>
-      <c r="E16">
-        <v>699</v>
-      </c>
-      <c r="F16">
-        <v>1216</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>10</v>
-      </c>
-      <c r="B17">
-        <v>4006</v>
-      </c>
-      <c r="C17">
-        <v>450</v>
-      </c>
-      <c r="E17">
-        <v>736</v>
-      </c>
-      <c r="F17">
-        <v>1370</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>11</v>
-      </c>
-      <c r="B18">
-        <v>4505</v>
-      </c>
-      <c r="C18">
-        <v>500</v>
-      </c>
-      <c r="E18">
+      <c r="D18" s="9">
         <v>828</v>
       </c>
-      <c r="F18">
+      <c r="E18" s="9">
         <v>1518</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
         <v>12</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="9">
         <v>5000</v>
       </c>
-      <c r="E19">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9">
         <v>918</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="E19" s="9"/>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
         <v>13</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="9">
         <v>5499</v>
       </c>
-      <c r="E20">
+      <c r="C20" s="9"/>
+      <c r="D20" s="9">
         <v>1009</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="E20" s="9"/>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
         <v>14</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="9">
         <v>6000</v>
       </c>
-      <c r="E21">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9">
         <v>1111</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="E21" s="9"/>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A22" s="9">
         <v>15</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="9">
         <v>6505</v>
       </c>
-      <c r="E22">
+      <c r="C22" s="9"/>
+      <c r="D22" s="9">
         <v>1197</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="E22" s="9"/>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A23" s="7">
         <v>16</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="7">
         <v>7006</v>
       </c>
-      <c r="E23">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7">
         <v>1284</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E23" s="7"/>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P32" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P34" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P35" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P36" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="P38" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C39" s="2">
         <v>3500</v>
       </c>
       <c r="D39" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="P39" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P40" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P41" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P42" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="P43" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P44" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P45" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A46" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3">
@@ -2061,10 +3736,13 @@
       <c r="L46" s="3">
         <v>10</v>
       </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P46" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="4">
@@ -2097,10 +3775,13 @@
       <c r="L47" s="4">
         <v>3557</v>
       </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="P47" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="5">
@@ -2147,10 +3828,13 @@
         <f>AVERAGE(C48:L48)</f>
         <v>-56.9</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="5">
@@ -2193,79 +3877,121 @@
         <f t="shared" si="1"/>
         <v>3249</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P49" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P50" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P51" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P52" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B53">
         <f>SUM(C49:L49)</f>
         <v>32389</v>
       </c>
       <c r="C53" t="s">
+        <v>13</v>
+      </c>
+      <c r="P53" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P54" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
         <v>14</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" t="s">
-        <v>15</v>
       </c>
       <c r="B55">
         <f>B53/9</f>
         <v>3598.7777777777778</v>
       </c>
       <c r="C55" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.2">
+        <v>13</v>
+      </c>
+      <c r="P55" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P56" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="P57" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B58">
         <f>SQRT(B55)</f>
         <v>59.989813950184725</v>
       </c>
       <c r="C58" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="P58" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B61">
         <f>1.96*B58</f>
         <v>117.58003534236207</v>
       </c>
       <c r="C61" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C65" s="2">
         <v>300</v>
       </c>
       <c r="D65" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B72" s="3"/>
       <c r="C72" s="3">
@@ -2301,7 +4027,7 @@
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="4">
@@ -2337,7 +4063,7 @@
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B74" s="3"/>
       <c r="C74" s="5">
@@ -2387,7 +4113,7 @@
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B75" s="3"/>
       <c r="C75" s="3">
@@ -2433,50 +4159,50 @@
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B79">
         <f>SUM(C75:L75)</f>
         <v>65</v>
       </c>
       <c r="C79" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B81">
         <f>B79/9</f>
         <v>7.2222222222222223</v>
       </c>
       <c r="C81" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B84">
         <f>SQRT(B81)</f>
         <v>2.6874192494328497</v>
       </c>
       <c r="C84" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B87">
         <f>1.96*B84</f>
         <v>5.2673417288883853</v>
       </c>
       <c r="C87" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -2485,4 +4211,19 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ikke funktionelle krav og accepttest for måleenhed
</commit_message>
<xml_diff>
--- a/Maaleenhed/Notater/3 maj - Volampere kredsløb/Kalibrering.xlsx
+++ b/Maaleenhed/Notater/3 maj - Volampere kredsløb/Kalibrering.xlsx
@@ -765,11 +765,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1078144720"/>
-        <c:axId val="1078147040"/>
+        <c:axId val="-14379648"/>
+        <c:axId val="-110440320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1078144720"/>
+        <c:axId val="-14379648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -896,12 +896,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078147040"/>
+        <c:crossAx val="-110440320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1078147040"/>
+        <c:axId val="-110440320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1028,7 +1028,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1078144720"/>
+        <c:crossAx val="-14379648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1574,11 +1574,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1161688096"/>
-        <c:axId val="1161690576"/>
+        <c:axId val="-14336368"/>
+        <c:axId val="-14333888"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1161688096"/>
+        <c:axId val="-14336368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1649,12 +1649,12 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1161690576"/>
+        <c:crossAx val="-14333888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1161690576"/>
+        <c:axId val="-14333888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1714,7 +1714,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1781,7 +1780,7 @@
             <a:endParaRPr lang="da-DK"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1161688096"/>
+        <c:crossAx val="-14336368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1795,7 +1794,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3312,8 +3310,8 @@
   <sheetPr codeName="Ark1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A3:P87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="P30" sqref="P30:P58"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="M78" sqref="M78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3892,6 +3890,10 @@
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M52">
+        <f>M48/C39*100</f>
+        <v>-1.6257142857142854</v>
+      </c>
       <c r="P52" t="s">
         <v>44</v>
       </c>
@@ -4155,6 +4157,12 @@
       <c r="L75" s="3">
         <f t="shared" si="3"/>
         <v>9</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="M77">
+        <f>M74/C65*100</f>
+        <v>-0.83333333333333337</v>
       </c>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>